<commit_message>
Add work with excel
</commit_message>
<xml_diff>
--- a/AutoMechanic/bin/Debug/Orders.xlsx
+++ b/AutoMechanic/bin/Debug/Orders.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\solov\source\repos\AutoMechanic\AutoMechanic\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D387917-14CB-4EEF-A021-1854E21EF7FB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C63F1B-C452-4902-80FC-A8F6272C0101}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,16 +33,16 @@
     <t>Bustrev</t>
   </si>
   <si>
-    <t>Жигуль</t>
-  </si>
-  <si>
     <t>а123бв</t>
   </si>
   <si>
     <t>Renault Logan</t>
   </si>
   <si>
-    <t>б228ох</t>
+    <t>BMW X5</t>
+  </si>
+  <si>
+    <t>е674ку</t>
   </si>
 </sst>
 </file>
@@ -363,12 +363,14 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="13.109375" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -382,10 +384,10 @@
         <v>89991231212</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -402,7 +404,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>